<commit_message>
change script to rpaframework
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -599,7 +599,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -636,26 +636,26 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Read Your Way Through Kerala</t>
+          <t>A Visa Backlog Abroad Is Taking a Toll Inside the U.S., Too</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>April 12, 2023</t>
+          <t>April 13, 2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A strip of lush land at the tip of India where spices grow wild, Kerala has long drawn the gaze of outsiders. Here’s Abraham Verghese’s guide to its literature, which nods at these influences but is very much its own.</t>
+          <t>The pileup has left visitors from places like Brazil, Colombia, India and Mexico waiting months, even a year or more, to visit family or do business in America.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/03/books/review/00LitGuide-KERALA/00LitGuide-KERALA-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/12/travel/12visa-backlog-illo/12visa-backlog-illo-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -664,7 +664,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>For Your Next Long Flight, Book a Couch in Coach</t>
+          <t>New Bargain Lodges Offer Rustic Comfort in the Heart of Nature</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -674,16 +674,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>An increasing number of long-haul airlines are offering economy seats that let passengers lie down. Sky couches as they’re often called, are a business-class approximation, without the frills, or the price.</t>
+          <t>From the Catskill Mountains in New York to the deserts of Utah, new or expanding hotel companies are creating affordable accommodations for those who love the outdoors.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/12/travel/12travel-sky-couch/12travel-sky-couch-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/10/travel/oakImage-1681159827777/oakImage-1681159827777-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -692,26 +692,26 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Passenger Flight Is Diverted After Woman Threatens Flight Attendant</t>
+          <t>Read Your Way Through Kerala</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>April 11, 2023</t>
+          <t>April 12, 2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>An Alaska Airlines flight from San Francisco to Chicago landed in Kansas City, Mo., after the passenger started acting erratically. She was arrested on a federal charge.</t>
+          <t>A strip of lush land at the tip of India where spices grow wild, Kerala has long drawn the gaze of outsiders. Here’s Abraham Verghese’s guide to its literature, which nods at these influences but is very much its own.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/11/multimedia/11xp-flight-bzfv/11xp-flight-bzfv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/03/books/review/00LitGuide-KERALA/00LitGuide-KERALA-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -720,26 +720,26 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Can Boracay Beat Overtourism?</t>
+          <t>For Your Next Long Flight, Book a Couch in Coach</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>April 11, 2023</t>
+          <t>April 12, 2023</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Called one of the world’s best islands, the Philippine resort was closed by the government for six months and reopened with a cap on visitors. Now, with travelers coming back, will it continue to hold the line?</t>
+          <t>An increasing number of long-haul airlines are offering economy seats that let passengers lie down. Sky couches as they’re often called, are a business-class approximation, without the frills, or the price.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/07/multimedia/00-boracay-philippines-gtcv/00-boracay-philippines-gtcv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/12/travel/12travel-sky-couch/12travel-sky-couch-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -748,26 +748,26 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Turning Over the Stones of England’s Lost Jewish Past</t>
+          <t>Passenger Flight Is Diverted After Woman Threatens Flight Attendant</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>April 10, 2023</t>
+          <t>April 11, 2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Around eight centuries ago, Jews thrived in England, worshiping freely and living where they pleased. Then everything changed. You can uncover their stories, if you know where to look.</t>
+          <t>An Alaska Airlines flight from San Francisco to Chicago landed in Kansas City, Mo., after the passenger started acting erratically. She was arrested on a federal charge.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/03/22/multimedia/00travel-jewishengland-gpbc/00travel-jewishengland-gpbc-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/11/multimedia/11xp-flight-bzfv/11xp-flight-bzfv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -776,26 +776,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Have Eggs, Will Travel. To Freeze Them.</t>
+          <t>Can Boracay Beat Overtourism?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>April 8, 2023</t>
+          <t>April 11, 2023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Faced with the high cost of egg-freezing in their home countries, some women are going abroad for a better deal, and a vacation.</t>
+          <t>Called one of the world’s best islands, the Philippine resort was closed by the government for six months and reopened with a cap on visitors. Now, with travelers coming back, will it continue to hold the line?</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/06/fashion/06EGG-FREEZING-TOURISM-top/06EGG-FREEZING-TOURISM-top-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/07/multimedia/00-boracay-philippines-gtcv/00-boracay-philippines-gtcv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -804,26 +804,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A Cobra Appeared Mid-Flight. The Pilot’s Quick Thinking Saved Lives.</t>
+          <t>Turning Over the Stones of England’s Lost Jewish Past</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>April 7, 2023</t>
+          <t>April 10, 2023</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The pilot made an emergency landing after feeling a Cape Cobra slither under his shirt while flying across South Africa. “I had a moment of stunned silence,” he said.</t>
+          <t>Around eight centuries ago, Jews thrived in England, worshiping freely and living where they pleased. Then everything changed. You can uncover their stories, if you know where to look.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/06/multimedia/07xp-plane-snake-bmfv/07xp-plane-snake-bmfv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/03/22/multimedia/00travel-jewishengland-gpbc/00travel-jewishengland-gpbc-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -832,26 +832,26 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A New Exhibition Shows That Barkley L. Hendricks Was Never Simply a Painter</t>
+          <t>Have Eggs, Will Travel. To Freeze Them.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>April 6, 2023</t>
+          <t>April 8, 2023</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Plus: an expanding group of Japanese restaurants in Brooklyn, exuberant tableware from Kit Kemp and more recommendations from T Magazine.</t>
+          <t>Faced with the high cost of egg-freezing in their home countries, some women are going abroad for a better deal, and a vacation.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/05/t-magazine/05tmag-newsletter-slide-TDQS/05tmag-newsletter-slide-TDQS-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/06/fashion/06EGG-FREEZING-TOURISM-top/06EGG-FREEZING-TOURISM-top-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -860,26 +860,26 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Booking the Paris Olympics for 2024? What You Need to Know.</t>
+          <t>A Cobra Appeared Mid-Flight. The Pilot’s Quick Thinking Saved Lives.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>April 6, 2023</t>
+          <t>April 7, 2023</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Next year’s Summer Olympic Games in Paris are expected to draw millions of spectators. Here’s how to get tickets if you want to be one of them.</t>
+          <t>The pilot made an emergency landing after feeling a Cape Cobra slither under his shirt while flying across South Africa. “I had a moment of stunned silence,” he said.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/04/multimedia/00travel-olympics-lbhc/00travel-olympics-lbhc-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/06/multimedia/07xp-plane-snake-bmfv/07xp-plane-snake-bmfv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -888,7 +888,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Dining in Style, at 90 Miles an Hour</t>
+          <t>A New Exhibition Shows That Barkley L. Hendricks Was Never Simply a Painter</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -898,16 +898,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Train travel is thriving in Central Europe, and so are dining cars. We rode the rails from Prague to Zurich and beyond, sampling regional dishes and savoring the views.</t>
+          <t>Plus: an expanding group of Japanese restaurants in Brooklyn, exuberant tableware from Kit Kemp and more recommendations from T Magazine.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/15/travel/05dining-cars-01-qfbv/05dining-cars-01-qfbv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/05/t-magazine/05tmag-newsletter-slide-TDQS/05tmag-newsletter-slide-TDQS-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -916,7 +916,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6 Picasso Shows to See This Year</t>
+          <t>Booking the Paris Olympics for 2024? What You Need to Know.</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -926,16 +926,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Fifty years after his death, the Cubist painter will be featured in art exhibitions in New York, Paris and Madrid.</t>
+          <t>Next year’s Summer Olympic Games in Paris are expected to draw millions of spectators. Here’s how to get tickets if you want to be one of them.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/09/multimedia/09picasso-list1-whmp/09picasso-list1-whmp-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/04/multimedia/00travel-olympics-lbhc/00travel-olympics-lbhc-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -944,7 +944,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>36 Hours in Tokyo</t>
+          <t>Dining in Style, at 90 Miles an Hour</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -954,16 +954,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Think of Tokyo as a warren of concealed gems: Wander down side streets and be richly rewarded.</t>
+          <t>Train travel is thriving in Central Europe, and so are dining cars. We rode the rails from Prague to Zurich and beyond, sampling regional dishes and savoring the views.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/06/multimedia/06hours-tokyo-ktzm/06hours-tokyo-ktzm-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/15/travel/05dining-cars-01-qfbv/05dining-cars-01-qfbv-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -972,26 +972,26 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>How to Brainstorm and Plan Events With Friends and Family</t>
+          <t>6 Picasso Shows to See This Year</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>April 5, 2023</t>
+          <t>April 6, 2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Many apps and tools for online collaboration work just as well for personal projects as they do for office tasks, and can be fun.</t>
+          <t>Fifty years after his death, the Cubist painter will be featured in art exhibitions in New York, Paris and Madrid.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/05/technology/personaltech/05TECHTIP-TOPART/05TECHTIP-TOPART-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/09/multimedia/09picasso-list1-whmp/09picasso-list1-whmp-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1000,26 +1000,26 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Fasten Your Seatbelts: What You Need to Know About Turbulence</t>
+          <t>36 Hours in Tokyo</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>April 5, 2023</t>
+          <t>April 6, 2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Recent incidents with turbulence during air travel raise questions about this challenging weather phenomenon. Here’s what we know about it and how to stay safe.</t>
+          <t>Think of Tokyo as a warren of concealed gems: Wander down side streets and be richly rewarded.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/07/travel/00travel-turbulence-illo/00travel-turbulence-illo-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/06/multimedia/06hours-tokyo-ktzm/06hours-tokyo-ktzm-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1028,7 +1028,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>If You Want to Learn Biathlon, Ski Fast and Stay Calm</t>
+          <t>How to Brainstorm and Plan Events With Friends and Family</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1038,16 +1038,16 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>At a former Olympic site in Utah, a first-timer finds that the sport, a hybrid of cross-country skiing and target shooting, requires serenity as well as speed.</t>
+          <t>Many apps and tools for online collaboration work just as well for personal projects as they do for office tasks, and can be fun.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/03/31/multimedia/00travel-biathlon-01-gfcm/00travel-biathlon-01-gfcm-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/05/technology/personaltech/05TECHTIP-TOPART/05TECHTIP-TOPART-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1056,7 +1056,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Help! My Dog Was Rejected by the Airline Because of a Carrier Rule That Doesn’t Exist.</t>
+          <t>Fasten Your Seatbelts: What You Need to Know About Turbulence</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1066,16 +1066,16 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>A gate agent suddenly objected to a canine who’d flown previously on the same route, saying the carrier wasn’t big enough. Our columnist tries to sort out what the actual rules for pets on planes are.</t>
+          <t>Recent incidents with turbulence during air travel raise questions about this challenging weather phenomenon. Here’s what we know about it and how to stay safe.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/04/travel/00tripped-up-illo/00tripped-up-illo-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/07/travel/00travel-turbulence-illo/00travel-turbulence-illo-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1084,26 +1084,26 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5 London Hotels Where You’ll Get the Royal Treatment</t>
+          <t>If You Want to Learn Biathlon, Ski Fast and Stay Calm</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>April 4, 2023</t>
+          <t>April 5, 2023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>If there was ever a time to splurge on a few days in the British capital, this is it. With the coronation approaching, here are some stylish places — old and new — where you can spend a certain weekend in May.</t>
+          <t>At a former Olympic site in Utah, a first-timer finds that the sport, a hybrid of cross-country skiing and target shooting, requires serenity as well as speed.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/03/31/travel/oakImage-1680266608174/oakImage-1680266608174-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/03/31/multimedia/00travel-biathlon-01-gfcm/00travel-biathlon-01-gfcm-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1112,26 +1112,26 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Hoping to Travel Abroad? Don’t Put Off Your Passport Application.</t>
+          <t>Help! My Dog Was Rejected by the Airline Because of a Carrier Rule That Doesn’t Exist.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>April 3, 2023</t>
+          <t>April 5, 2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Processing times for new and renewed passports have increased again. The updated timeline, 10 to 13 weeks, leaves some would-be travelers feeling desperate.</t>
+          <t>A gate agent suddenly objected to a canine who’d flown previously on the same route, saying the carrier wasn’t big enough. Our columnist tries to sort out what the actual rules for pets on planes are.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/04/06/multimedia/06travel-passports-1-vmlh/06travel-passports-1-vmlh-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/04/04/travel/00tripped-up-illo/00tripped-up-illo-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1140,26 +1140,26 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Thailand’s Unemployed Elephants Are Back Home, Huge and Hungry</t>
+          <t>5 London Hotels Where You’ll Get the Royal Treatment</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>April 1, 2023</t>
+          <t>April 4, 2023</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>When the tourists who rode them disappeared from resort destinations, Thailand’s captive elephants, and their owners, went back to their birth villages, where finding enough food has been a struggle.</t>
+          <t>If there was ever a time to splurge on a few days in the British capital, this is it. With the coronation approaching, here are some stylish places — old and new — where you can spend a certain weekend in May.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://static01.nyt.com/images/2023/03/23/multimedia/00thailand-elephant-dispatch-01-zchl/00thailand-elephant-dispatch-01-zchl-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+          <t>https://static01.nyt.com/images/2023/03/31/travel/oakImage-1680266608174/oakImage-1680266608174-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1168,28 +1168,84 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>Hoping to Travel Abroad? Don’t Put Off Your Passport Application.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>April 3, 2023</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Processing times for new and renewed passports have increased again. The updated timeline, 10 to 13 weeks, leaves some would-be travelers feeling desperate.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://static01.nyt.com/images/2023/04/06/multimedia/06travel-passports-1-vmlh/06travel-passports-1-vmlh-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Thailand’s Unemployed Elephants Are Back Home, Huge and Hungry</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>April 1, 2023</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>When the tourists who rode them disappeared from resort destinations, Thailand’s captive elephants, and their owners, went back to their birth villages, where finding enough food has been a struggle.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://static01.nyt.com/images/2023/03/23/multimedia/00thailand-elephant-dispatch-01-zchl/00thailand-elephant-dispatch-01-zchl-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>10 Places to See Wildflowers in the West</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>April 1, 2023</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>A ‘super bloom’ may be in the eye of the beholder, but the winter’s rain and snow promises a bumper crop of spring blooms in Southern California and Arizona.</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>https://static01.nyt.com/images/2023/04/15/travel/00-spring-wildflowers-thqm/00-spring-wildflowers-thqm-thumbWide.jpg?quality=75&amp;auto=webp&amp;disable=upscale</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>9</v>
-      </c>
-      <c r="F27" t="b">
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>